<commit_message>
presentation and data, which was done last night
</commit_message>
<xml_diff>
--- a/presentation/data.xlsx
+++ b/presentation/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22640" tabRatio="500"/>
+    <workbookView xWindow="15500" yWindow="0" windowWidth="22900" windowHeight="22640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Filename</t>
   </si>
@@ -53,12 +53,33 @@
   <si>
     <t>sadness</t>
   </si>
+  <si>
+    <t>glory(norm)</t>
+  </si>
+  <si>
+    <t>affection(norm)</t>
+  </si>
+  <si>
+    <t>aggression(norm)</t>
+  </si>
+  <si>
+    <t>anxiety(norm)</t>
+  </si>
+  <si>
+    <t>sadness(norm)</t>
+  </si>
+  <si>
+    <t>expressive behavior(norm)</t>
+  </si>
+  <si>
+    <t>positive affect(norm)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -98,6 +119,11 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -122,20 +148,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -500,11 +547,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2081385624"/>
-        <c:axId val="-2077697544"/>
+        <c:axId val="2112218312"/>
+        <c:axId val="2112221288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2081385624"/>
+        <c:axId val="2112218312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -513,7 +560,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2077697544"/>
+        <c:crossAx val="2112221288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -521,7 +568,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2077697544"/>
+        <c:axId val="2112221288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -532,7 +579,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2081385624"/>
+        <c:crossAx val="2112218312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -570,7 +617,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0317136121457872"/>
+          <c:y val="0.039647577092511"/>
+          <c:w val="0.801819321985949"/>
+          <c:h val="0.915536092129453"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1347,11 +1404,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2077457112"/>
-        <c:axId val="-2077455144"/>
+        <c:axId val="2112300680"/>
+        <c:axId val="2112303656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2077457112"/>
+        <c:axId val="2112300680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1360,7 +1417,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2077455144"/>
+        <c:crossAx val="2112303656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1368,7 +1425,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2077455144"/>
+        <c:axId val="2112303656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1379,7 +1436,1760 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2077457112"/>
+        <c:crossAx val="2112300680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>glory(norm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$2:$L$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.016968</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.028543</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.009091</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.015428</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.021438</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.025882</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.013289</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.024091</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.019802</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0061</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.022463</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.028603</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.031517</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.015825</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.014496</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.00576</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.014952</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.007837</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.046237</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.018001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.031126</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.015848</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.017512</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.005894</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.011201</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.046653</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.033062</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>affection(norm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.021493</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.007874</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01039</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.008415</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.002522</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.002353</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.006645</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.005668</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.01273</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.007843</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.012393</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.005134</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.005876</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.005387</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.008065</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.000576</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.00589</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.010972</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.013967</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.004552</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.008772</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.004754</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.012681</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.00943</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.009857</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.009414</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.010149</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>aggression(norm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$2:$N$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.002262</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.026575</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.012987</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.008415</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01261</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.014118</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.013289</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.008975</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.024045</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.007407</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.013943</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.015035</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.019765</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.011785</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.009187</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.019009</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.017218</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.010188</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.012282</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.009518</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.009621</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.009509</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.003623</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.01611</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.009857</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.011088</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.008611</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>positive affect(norm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$2:$O$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.003394</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.001969</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.009091</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.002805</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.001261</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.007059</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.001889</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.008487</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.008715</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.002324</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.002567</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.004808</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.005724</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.006329</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.001728</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.004531</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.00627</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.00602</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.003311</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.003396</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.001585</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.004227</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.004715</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.002688</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.00523</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.003076</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>anxiety(norm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$2:$Q$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.011312</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00689</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.001403</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.006305</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.002353</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.004251</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.001414</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.001307</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.006197</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.005134</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.007479</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.005724</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.006635</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.004032</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.003172</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.000784</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.003492</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.001655</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.003396</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.00317</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.001208</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.004715</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.001344</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.003766</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.003383</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sadness(norm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.011312</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.009843</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.002597</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.001403</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.005044</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.009967</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.003307</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.008487</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.00305</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.003873</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0022</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.009615</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.004377</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.003879</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.004032</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.003625</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.000784</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.003853</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.003104</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.004527</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.00317</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.005435</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.001965</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.001344</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.003766</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.002153</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>expressive behavior(norm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$2:$R$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.005656</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.002953</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.005195</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.006305</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.009412</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.005196</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.005658</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.007843</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.003098</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.008067</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.005342</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.005051</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.003675</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.006336</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.003625</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.007837</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.005418</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.005587</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.004244</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.004831</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.003929</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.004928</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.003766</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2132189576"/>
+        <c:axId val="2135252600"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2132189576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2135252600"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2135252600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2132189576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>affection(norm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.021493</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.007874</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01039</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.008415</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.002522</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.002353</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.006645</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.005668</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.01273</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.007843</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.012393</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.005134</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.005876</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.005387</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.008065</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.000576</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.00589</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.010972</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.013967</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.004552</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.008772</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.004754</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.012681</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.00943</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.009857</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.009414</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.010149</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>aggression(norm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$2:$N$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.002262</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.026575</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.012987</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.008415</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01261</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.014118</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.013289</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.008975</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.024045</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.007407</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.013943</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.015035</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.019765</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.011785</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.009187</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.019009</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.017218</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.010188</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.012282</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.009518</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.009621</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.009509</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.003623</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.01611</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.009857</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.011088</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.008611</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2138149864"/>
+        <c:axId val="2138135720"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2138149864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2138135720"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2138135720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2138149864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>positive affect(norm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$2:$O$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.003394</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.001969</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.009091</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.002805</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.001261</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.007059</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.001889</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.008487</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.008715</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.002324</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.002567</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.004808</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.005724</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.006329</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.001728</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.004531</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.00627</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.00602</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.003311</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.003396</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.001585</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.004227</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.004715</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.002688</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.00523</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.003076</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sadness(norm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.011312</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.009843</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.002597</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.001403</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.005044</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.009967</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.003307</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.008487</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.00305</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.003873</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0022</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.009615</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.004377</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.003879</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.004032</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.003625</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.000784</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.003853</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.003104</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.004527</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.00317</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.005435</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.001965</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.001344</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.003766</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.002153</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2138607496"/>
+        <c:axId val="2140014888"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2138607496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2140014888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2140014888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2138607496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>anxiety(norm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$2:$Q$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.011312</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00689</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.001403</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.006305</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.002353</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.004251</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.001414</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.001307</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.006197</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.005134</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.007479</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.005724</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.006635</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.004032</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.003172</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.000784</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.003492</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.001655</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.003396</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.00317</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.001208</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.004715</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.001344</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.003766</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.003383</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>expressive behavior(norm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$2:$R$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.005656</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.002953</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.005195</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.006305</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.009412</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.005196</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.005658</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.007843</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.003098</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.008067</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.005342</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.005051</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.003675</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.006336</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.003625</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.007837</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.005418</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.005587</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.004244</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.004831</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.003929</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.004928</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.003766</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2146281880"/>
+        <c:axId val="2140099704"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2146281880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2140099704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2140099704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2146281880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1405,16 +3215,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1435,16 +3245,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1498600</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1458,6 +3268,126 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1485900</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1308100</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1788,10 +3718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="L149" sqref="L149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1805,9 +3735,16 @@
     <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="21.83203125" customWidth="1"/>
     <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
+    <col min="13" max="13" width="22.6640625" customWidth="1"/>
+    <col min="14" max="14" width="22.83203125" customWidth="1"/>
+    <col min="15" max="15" width="28.83203125" customWidth="1"/>
+    <col min="16" max="16" width="19.5" customWidth="1"/>
+    <col min="17" max="17" width="24.6640625" customWidth="1"/>
+    <col min="18" max="18" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="23">
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="23">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1841,8 +3778,29 @@
       <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="20">
+    <row r="2" spans="1:18" ht="20">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1876,8 +3834,29 @@
       <c r="K2">
         <v>10</v>
       </c>
+      <c r="L2" s="4">
+        <v>1.6968E-2</v>
+      </c>
+      <c r="M2" s="4">
+        <v>2.1493000000000002E-2</v>
+      </c>
+      <c r="N2" s="4">
+        <v>2.2620000000000001E-3</v>
+      </c>
+      <c r="O2" s="4">
+        <v>3.3939999999999999E-3</v>
+      </c>
+      <c r="P2" s="4">
+        <v>1.1311999999999999E-2</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>1.1311999999999999E-2</v>
+      </c>
+      <c r="R2" s="4">
+        <v>5.6559999999999996E-3</v>
+      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:18" ht="16">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1911,8 +3890,29 @@
       <c r="K3">
         <v>10</v>
       </c>
+      <c r="L3" s="4">
+        <v>2.8542999999999999E-2</v>
+      </c>
+      <c r="M3" s="4">
+        <v>7.8740000000000008E-3</v>
+      </c>
+      <c r="N3" s="4">
+        <v>2.6575000000000001E-2</v>
+      </c>
+      <c r="O3" s="4">
+        <v>1.9689999999999998E-3</v>
+      </c>
+      <c r="P3" s="4">
+        <v>9.8429999999999993E-3</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>6.8900000000000003E-3</v>
+      </c>
+      <c r="R3" s="4">
+        <v>2.9529999999999999E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:18" ht="16">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1946,8 +3946,29 @@
       <c r="K4" s="2">
         <v>2</v>
       </c>
+      <c r="L4" s="4">
+        <v>9.0910000000000001E-3</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1.039E-2</v>
+      </c>
+      <c r="N4" s="4">
+        <v>1.2987E-2</v>
+      </c>
+      <c r="O4" s="4">
+        <v>9.0910000000000001E-3</v>
+      </c>
+      <c r="P4" s="4">
+        <v>2.5969999999999999E-3</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>0</v>
+      </c>
+      <c r="R4" s="4">
+        <v>5.195E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:18" ht="16">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1981,8 +4002,29 @@
       <c r="K5" s="2">
         <v>1</v>
       </c>
+      <c r="L5" s="4">
+        <v>1.5428000000000001E-2</v>
+      </c>
+      <c r="M5" s="4">
+        <v>8.4150000000000006E-3</v>
+      </c>
+      <c r="N5" s="4">
+        <v>8.4150000000000006E-3</v>
+      </c>
+      <c r="O5" s="4">
+        <v>2.8050000000000002E-3</v>
+      </c>
+      <c r="P5" s="4">
+        <v>1.403E-3</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>1.403E-3</v>
+      </c>
+      <c r="R5" s="4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:18" ht="16">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2016,8 +4058,29 @@
       <c r="K6">
         <v>4</v>
       </c>
+      <c r="L6" s="4">
+        <v>2.1437999999999999E-2</v>
+      </c>
+      <c r="M6" s="4">
+        <v>2.5219999999999999E-3</v>
+      </c>
+      <c r="N6" s="4">
+        <v>1.261E-2</v>
+      </c>
+      <c r="O6" s="4">
+        <v>1.261E-3</v>
+      </c>
+      <c r="P6" s="4">
+        <v>5.0439999999999999E-3</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>6.3049999999999998E-3</v>
+      </c>
+      <c r="R6" s="4">
+        <v>6.3049999999999998E-3</v>
+      </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:18" ht="16">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2051,8 +4114,29 @@
       <c r="K7" s="2">
         <v>0</v>
       </c>
+      <c r="L7" s="4">
+        <v>2.5881999999999999E-2</v>
+      </c>
+      <c r="M7" s="4">
+        <v>2.3530000000000001E-3</v>
+      </c>
+      <c r="N7" s="4">
+        <v>1.4118E-2</v>
+      </c>
+      <c r="O7" s="4">
+        <v>7.0590000000000002E-3</v>
+      </c>
+      <c r="P7" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>2.3530000000000001E-3</v>
+      </c>
+      <c r="R7" s="4">
+        <v>9.4120000000000002E-3</v>
+      </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:18" ht="16">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2086,8 +4170,29 @@
       <c r="K8" s="2">
         <v>3</v>
       </c>
+      <c r="L8" s="4">
+        <v>1.3289E-2</v>
+      </c>
+      <c r="M8" s="4">
+        <v>6.6449999999999999E-3</v>
+      </c>
+      <c r="N8" s="4">
+        <v>1.3289E-2</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0</v>
+      </c>
+      <c r="P8" s="4">
+        <v>9.9670000000000002E-3</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>0</v>
+      </c>
+      <c r="R8" s="4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:18" ht="16">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2121,8 +4226,29 @@
       <c r="K9" s="2">
         <v>7</v>
       </c>
+      <c r="L9" s="4">
+        <v>2.4091000000000001E-2</v>
+      </c>
+      <c r="M9" s="4">
+        <v>5.6680000000000003E-3</v>
+      </c>
+      <c r="N9" s="4">
+        <v>8.9750000000000003E-3</v>
+      </c>
+      <c r="O9" s="4">
+        <v>1.8890000000000001E-3</v>
+      </c>
+      <c r="P9" s="4">
+        <v>3.307E-3</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>4.2509999999999996E-3</v>
+      </c>
+      <c r="R9" s="4">
+        <v>5.1960000000000001E-3</v>
+      </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:18" ht="16">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2156,8 +4282,29 @@
       <c r="K10" s="2">
         <v>6</v>
       </c>
+      <c r="L10" s="4">
+        <v>1.9802E-2</v>
+      </c>
+      <c r="M10" s="4">
+        <v>1.273E-2</v>
+      </c>
+      <c r="N10" s="4">
+        <v>2.4045E-2</v>
+      </c>
+      <c r="O10" s="4">
+        <v>8.4869999999999998E-3</v>
+      </c>
+      <c r="P10" s="4">
+        <v>8.4869999999999998E-3</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>1.4139999999999999E-3</v>
+      </c>
+      <c r="R10" s="4">
+        <v>5.6579999999999998E-3</v>
+      </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:18" ht="16">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2191,8 +4338,29 @@
       <c r="K11" s="2">
         <v>7</v>
       </c>
+      <c r="L11" s="4">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="M11" s="4">
+        <v>7.8429999999999993E-3</v>
+      </c>
+      <c r="N11" s="4">
+        <v>7.4070000000000004E-3</v>
+      </c>
+      <c r="O11" s="4">
+        <v>8.7150000000000005E-3</v>
+      </c>
+      <c r="P11" s="4">
+        <v>3.0500000000000002E-3</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>1.307E-3</v>
+      </c>
+      <c r="R11" s="4">
+        <v>7.8429999999999993E-3</v>
+      </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:18" ht="16">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2226,8 +4394,29 @@
       <c r="K12" s="2">
         <v>5</v>
       </c>
+      <c r="L12" s="4">
+        <v>2.2463E-2</v>
+      </c>
+      <c r="M12" s="4">
+        <v>1.2393E-2</v>
+      </c>
+      <c r="N12" s="4">
+        <v>1.3943000000000001E-2</v>
+      </c>
+      <c r="O12" s="4">
+        <v>2.3240000000000001E-3</v>
+      </c>
+      <c r="P12" s="4">
+        <v>3.8730000000000001E-3</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>6.1970000000000003E-3</v>
+      </c>
+      <c r="R12" s="4">
+        <v>3.0980000000000001E-3</v>
+      </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:18" ht="16">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2261,8 +4450,29 @@
       <c r="K13" s="2">
         <v>6</v>
       </c>
+      <c r="L13" s="4">
+        <v>2.8603E-2</v>
+      </c>
+      <c r="M13" s="4">
+        <v>5.1339999999999997E-3</v>
+      </c>
+      <c r="N13" s="4">
+        <v>1.5035E-2</v>
+      </c>
+      <c r="O13" s="4">
+        <v>2.5669999999999998E-3</v>
+      </c>
+      <c r="P13" s="4">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>5.1339999999999997E-3</v>
+      </c>
+      <c r="R13" s="4">
+        <v>8.0669999999999995E-3</v>
+      </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:18" ht="16">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2296,8 +4506,29 @@
       <c r="K14" s="2">
         <v>18</v>
       </c>
+      <c r="L14" s="4">
+        <v>3.1517000000000003E-2</v>
+      </c>
+      <c r="M14" s="4">
+        <v>5.8760000000000001E-3</v>
+      </c>
+      <c r="N14" s="4">
+        <v>1.9765000000000001E-2</v>
+      </c>
+      <c r="O14" s="4">
+        <v>4.8079999999999998E-3</v>
+      </c>
+      <c r="P14" s="4">
+        <v>9.6150000000000003E-3</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>7.4790000000000004E-3</v>
+      </c>
+      <c r="R14" s="4">
+        <v>5.3420000000000004E-3</v>
+      </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:18" ht="16">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2331,8 +4562,29 @@
       <c r="K15" s="2">
         <v>13</v>
       </c>
+      <c r="L15" s="4">
+        <v>1.5824999999999999E-2</v>
+      </c>
+      <c r="M15" s="4">
+        <v>5.3870000000000003E-3</v>
+      </c>
+      <c r="N15" s="4">
+        <v>1.1785E-2</v>
+      </c>
+      <c r="O15" s="4">
+        <v>5.7239999999999999E-3</v>
+      </c>
+      <c r="P15" s="4">
+        <v>4.3769999999999998E-3</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>5.7239999999999999E-3</v>
+      </c>
+      <c r="R15" s="4">
+        <v>5.0509999999999999E-3</v>
+      </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:18" ht="16">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2366,8 +4618,29 @@
       <c r="K16" s="2">
         <v>38</v>
       </c>
+      <c r="L16" s="4">
+        <v>1.4496E-2</v>
+      </c>
+      <c r="M16" s="4">
+        <v>8.0649999999999993E-3</v>
+      </c>
+      <c r="N16" s="4">
+        <v>9.1870000000000007E-3</v>
+      </c>
+      <c r="O16" s="4">
+        <v>6.3290000000000004E-3</v>
+      </c>
+      <c r="P16" s="4">
+        <v>3.8790000000000001E-3</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>6.6350000000000003E-3</v>
+      </c>
+      <c r="R16" s="4">
+        <v>3.6749999999999999E-3</v>
+      </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:18" ht="16">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2401,8 +4674,29 @@
       <c r="K17" s="2">
         <v>7</v>
       </c>
+      <c r="L17" s="4">
+        <v>5.7600000000000004E-3</v>
+      </c>
+      <c r="M17" s="4">
+        <v>5.7600000000000001E-4</v>
+      </c>
+      <c r="N17" s="4">
+        <v>1.9009000000000002E-2</v>
+      </c>
+      <c r="O17" s="4">
+        <v>1.7279999999999999E-3</v>
+      </c>
+      <c r="P17" s="4">
+        <v>4.032E-3</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>4.032E-3</v>
+      </c>
+      <c r="R17" s="4">
+        <v>6.3359999999999996E-3</v>
+      </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:18" ht="16">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2436,8 +4730,29 @@
       <c r="K18" s="2">
         <v>8</v>
       </c>
+      <c r="L18" s="4">
+        <v>1.4952E-2</v>
+      </c>
+      <c r="M18" s="4">
+        <v>5.8900000000000003E-3</v>
+      </c>
+      <c r="N18" s="4">
+        <v>1.7218000000000001E-2</v>
+      </c>
+      <c r="O18" s="4">
+        <v>4.5310000000000003E-3</v>
+      </c>
+      <c r="P18" s="4">
+        <v>3.6250000000000002E-3</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>3.1719999999999999E-3</v>
+      </c>
+      <c r="R18" s="4">
+        <v>3.6250000000000002E-3</v>
+      </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:18" ht="16">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2471,8 +4786,29 @@
       <c r="K19" s="2">
         <v>1</v>
       </c>
+      <c r="L19" s="4">
+        <v>7.8370000000000002E-3</v>
+      </c>
+      <c r="M19" s="4">
+        <v>1.0972000000000001E-2</v>
+      </c>
+      <c r="N19" s="4">
+        <v>1.0187999999999999E-2</v>
+      </c>
+      <c r="O19" s="4">
+        <v>6.2700000000000004E-3</v>
+      </c>
+      <c r="P19" s="4">
+        <v>7.8399999999999997E-4</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>7.8399999999999997E-4</v>
+      </c>
+      <c r="R19" s="4">
+        <v>7.8370000000000002E-3</v>
+      </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:18" ht="16">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2506,8 +4842,29 @@
       <c r="K20" s="2">
         <v>32</v>
       </c>
+      <c r="L20" s="4">
+        <v>4.6237E-2</v>
+      </c>
+      <c r="M20" s="4">
+        <v>1.3967E-2</v>
+      </c>
+      <c r="N20" s="4">
+        <v>1.2282E-2</v>
+      </c>
+      <c r="O20" s="4">
+        <v>6.0200000000000002E-3</v>
+      </c>
+      <c r="P20" s="4">
+        <v>3.8530000000000001E-3</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>3.4919999999999999E-3</v>
+      </c>
+      <c r="R20" s="4">
+        <v>5.4180000000000001E-3</v>
+      </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:18" ht="16">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2541,8 +4898,29 @@
       <c r="K21" s="2">
         <v>15</v>
       </c>
+      <c r="L21" s="4">
+        <v>1.8001E-2</v>
+      </c>
+      <c r="M21" s="4">
+        <v>4.5519999999999996E-3</v>
+      </c>
+      <c r="N21" s="4">
+        <v>9.5180000000000004E-3</v>
+      </c>
+      <c r="O21" s="4">
+        <v>3.3110000000000001E-3</v>
+      </c>
+      <c r="P21" s="4">
+        <v>3.104E-3</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>1.655E-3</v>
+      </c>
+      <c r="R21" s="4">
+        <v>5.587E-3</v>
+      </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:18" ht="16">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2576,8 +4954,29 @@
       <c r="K22" s="2">
         <v>16</v>
       </c>
+      <c r="L22" s="4">
+        <v>3.1126000000000001E-2</v>
+      </c>
+      <c r="M22" s="4">
+        <v>8.7720000000000003E-3</v>
+      </c>
+      <c r="N22" s="4">
+        <v>9.6209999999999993E-3</v>
+      </c>
+      <c r="O22" s="4">
+        <v>3.3960000000000001E-3</v>
+      </c>
+      <c r="P22" s="4">
+        <v>4.5269999999999998E-3</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>3.3960000000000001E-3</v>
+      </c>
+      <c r="R22" s="4">
+        <v>4.2440000000000004E-3</v>
+      </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:18" ht="16">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2611,8 +5010,29 @@
       <c r="K23" s="2">
         <v>2</v>
       </c>
+      <c r="L23" s="4">
+        <v>1.5848000000000001E-2</v>
+      </c>
+      <c r="M23" s="4">
+        <v>4.7540000000000004E-3</v>
+      </c>
+      <c r="N23" s="4">
+        <v>9.5090000000000001E-3</v>
+      </c>
+      <c r="O23" s="4">
+        <v>1.585E-3</v>
+      </c>
+      <c r="P23" s="4">
+        <v>3.1700000000000001E-3</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>3.1700000000000001E-3</v>
+      </c>
+      <c r="R23" s="4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:18" ht="16">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2646,8 +5066,29 @@
       <c r="K24" s="2">
         <v>9</v>
       </c>
+      <c r="L24" s="4">
+        <v>1.7512E-2</v>
+      </c>
+      <c r="M24" s="4">
+        <v>1.2681E-2</v>
+      </c>
+      <c r="N24" s="4">
+        <v>3.6229999999999999E-3</v>
+      </c>
+      <c r="O24" s="4">
+        <v>4.2269999999999999E-3</v>
+      </c>
+      <c r="P24" s="4">
+        <v>5.4349999999999997E-3</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>1.2080000000000001E-3</v>
+      </c>
+      <c r="R24" s="4">
+        <v>4.8310000000000002E-3</v>
+      </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:18" ht="16">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2681,8 +5122,29 @@
       <c r="K25" s="2">
         <v>5</v>
       </c>
+      <c r="L25" s="4">
+        <v>5.8939999999999999E-3</v>
+      </c>
+      <c r="M25" s="4">
+        <v>9.4299999999999991E-3</v>
+      </c>
+      <c r="N25" s="4">
+        <v>1.6109999999999999E-2</v>
+      </c>
+      <c r="O25" s="4">
+        <v>4.7149999999999996E-3</v>
+      </c>
+      <c r="P25" s="4">
+        <v>1.9650000000000002E-3</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>4.7149999999999996E-3</v>
+      </c>
+      <c r="R25" s="4">
+        <v>3.9290000000000002E-3</v>
+      </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:18" ht="16">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2716,8 +5178,29 @@
       <c r="K26" s="2">
         <v>3</v>
       </c>
+      <c r="L26" s="4">
+        <v>1.1200999999999999E-2</v>
+      </c>
+      <c r="M26" s="4">
+        <v>9.8569999999999994E-3</v>
+      </c>
+      <c r="N26" s="4">
+        <v>9.8569999999999994E-3</v>
+      </c>
+      <c r="O26" s="4">
+        <v>2.6879999999999999E-3</v>
+      </c>
+      <c r="P26" s="4">
+        <v>1.3439999999999999E-3</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>1.3439999999999999E-3</v>
+      </c>
+      <c r="R26" s="4">
+        <v>4.9280000000000001E-3</v>
+      </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:18" ht="16">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2751,8 +5234,29 @@
       <c r="K27" s="2">
         <v>18</v>
       </c>
+      <c r="L27" s="4">
+        <v>4.6653E-2</v>
+      </c>
+      <c r="M27" s="4">
+        <v>9.4140000000000005E-3</v>
+      </c>
+      <c r="N27" s="4">
+        <v>1.1088000000000001E-2</v>
+      </c>
+      <c r="O27" s="4">
+        <v>5.2300000000000003E-3</v>
+      </c>
+      <c r="P27" s="4">
+        <v>3.7659999999999998E-3</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>3.7659999999999998E-3</v>
+      </c>
+      <c r="R27" s="4">
+        <v>3.7659999999999998E-3</v>
+      </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:18" ht="16">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2785,6 +5289,27 @@
       </c>
       <c r="K28" s="2">
         <v>14</v>
+      </c>
+      <c r="L28" s="4">
+        <v>3.3062000000000001E-2</v>
+      </c>
+      <c r="M28" s="4">
+        <v>1.0149E-2</v>
+      </c>
+      <c r="N28" s="4">
+        <v>8.6110000000000006E-3</v>
+      </c>
+      <c r="O28" s="4">
+        <v>3.0760000000000002E-3</v>
+      </c>
+      <c r="P28" s="4">
+        <v>2.153E-3</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>3.3830000000000002E-3</v>
+      </c>
+      <c r="R28" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>